<commit_message>
second commit upto doc and main error recove
</commit_message>
<xml_diff>
--- a/Student_data.xlsx
+++ b/Student_data.xlsx
@@ -524,7 +524,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>8000</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1555</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -559,7 +559,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>dhp</t>
+          <t>vhjvh</t>
         </is>
       </c>
     </row>

</xml_diff>